<commit_message>
SPI ~ GDP & SPI ~ LnGDP visualization
</commit_message>
<xml_diff>
--- a/SPI - graph and regression/data.xlsx
+++ b/SPI - graph and regression/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fangxiaoling/Documents/Nathan Nunn RA/Book/SPI - graph and regression/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8AC5F2-AC6D-A142-9D37-E971E7479B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBBBA9E-3D8A-7B4D-8579-983DD85EF64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" xr2:uid="{759FBD81-29F0-F145-96FE-6E13E18CF612}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="346">
   <si>
     <t>code</t>
   </si>
@@ -1067,13 +1067,13 @@
     <t>Palestine</t>
   </si>
   <si>
-    <t>\</t>
-  </si>
-  <si>
     <t>KR</t>
   </si>
   <si>
     <t>South Korea</t>
+  </si>
+  <si>
+    <t>logG_2025</t>
   </si>
 </sst>
 </file>
@@ -1115,9 +1115,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1452,15 +1457,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DF2D50-9E36-F54F-8776-CA765C779046}">
-  <dimension ref="A1:E171"/>
+  <dimension ref="A1:F171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="267" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView tabSelected="1" zoomScale="267" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="15.1640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1474,10 +1484,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1490,11 +1503,15 @@
       <c r="D2" s="1">
         <v>71224.34</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
+        <f>LN(D2)</f>
+        <v>11.17358989291391</v>
+      </c>
+      <c r="F2" s="1">
         <v>90.54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1507,11 +1524,15 @@
       <c r="D3" s="1">
         <v>88711.99</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E66" si="0">LN(D3)</f>
+        <v>11.393150333908723</v>
+      </c>
+      <c r="F3" s="1">
         <v>90.74</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1524,11 +1545,15 @@
       <c r="D4" s="1">
         <v>58634.37</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>10.979076322401525</v>
+      </c>
+      <c r="F4" s="1">
         <v>90.46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1541,11 +1566,15 @@
       <c r="D5" s="1">
         <v>64778.01</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>11.078721472895644</v>
+      </c>
+      <c r="F5" s="1">
         <v>89.42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1558,11 +1587,15 @@
       <c r="D6" s="1">
         <v>83019.839999999997</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>11.326834894358726</v>
+      </c>
+      <c r="F6" s="1">
         <v>90.26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1575,11 +1608,15 @@
       <c r="D7" s="1">
         <v>64294.75</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>11.071233258369737</v>
+      </c>
+      <c r="F7" s="1">
         <v>89.54</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1592,11 +1629,15 @@
       <c r="D8" s="1">
         <v>69953.67</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>11.15558844476451</v>
+      </c>
+      <c r="F8" s="1">
         <v>88.97</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1609,11 +1650,15 @@
       <c r="D9" s="1">
         <v>122595.8</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>11.716648044148661</v>
+      </c>
+      <c r="F9" s="1">
         <v>87.69</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -1626,11 +1671,15 @@
       <c r="D10" s="1">
         <v>137059.19</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>11.828168155301835</v>
+      </c>
+      <c r="F10" s="1">
         <v>87.48</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1643,11 +1692,15 @@
       <c r="D11" s="1">
         <v>62605.47</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>11.044607933462457</v>
+      </c>
+      <c r="F11" s="1">
         <v>88.72</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1660,11 +1713,15 @@
       <c r="D12" s="1">
         <v>65836.89</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>11.094935598512345</v>
+      </c>
+      <c r="F12" s="1">
         <v>88.05</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -1677,11 +1734,15 @@
       <c r="D13" s="1">
         <v>59119.98</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>10.987324217327034</v>
+      </c>
+      <c r="F13" s="1">
         <v>87.83</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -1694,11 +1755,15 @@
       <c r="D14" s="1">
         <v>63431.05</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>11.057708768172155</v>
+      </c>
+      <c r="F14" s="1">
         <v>87.22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -1711,11 +1776,15 @@
       <c r="D15" s="1">
         <v>44913.77</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>10.712499708227659</v>
+      </c>
+      <c r="F15" s="1">
         <v>88.19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1728,11 +1797,15 @@
       <c r="D16" s="1">
         <v>129038.47</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>11.767865855940206</v>
+      </c>
+      <c r="F16" s="1">
         <v>83.76</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1745,11 +1818,15 @@
       <c r="D17" s="1">
         <v>43877</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>10.68914554377483</v>
+      </c>
+      <c r="F17" s="1">
         <v>86.16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
@@ -1762,11 +1839,15 @@
       <c r="D18" s="1">
         <v>47558.27</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>10.769710975037997</v>
+      </c>
+      <c r="F18" s="1">
         <v>84.19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
@@ -1779,11 +1860,15 @@
       <c r="D19" s="1">
         <v>56716.37</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>10.94581816056845</v>
+      </c>
+      <c r="F19" s="1">
         <v>88.17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1796,11 +1881,15 @@
       <c r="D20" s="1">
         <v>49816.14</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>10.816094306890397</v>
+      </c>
+      <c r="F20" s="1">
         <v>87.26</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -1813,11 +1902,15 @@
       <c r="D21" s="1">
         <v>55183.63</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>10.918421630312162</v>
+      </c>
+      <c r="F21" s="1">
         <v>86.13</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -1830,11 +1923,15 @@
       <c r="D22" s="1">
         <v>45787.7</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="2">
+        <f t="shared" si="0"/>
+        <v>10.731770775081898</v>
+      </c>
+      <c r="F22" s="1">
         <v>85.35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -1847,11 +1944,15 @@
       <c r="D23" s="1">
         <v>48783.99</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>10.795157464242774</v>
+      </c>
+      <c r="F23" s="1">
         <v>85.19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -1864,11 +1965,15 @@
       <c r="D24" s="1">
         <v>54988.33</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>10.91487625988268</v>
+      </c>
+      <c r="F24" s="1">
         <v>86.07</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -1881,11 +1986,15 @@
       <c r="D25" s="1">
         <v>41240.39</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>10.627173394924203</v>
+      </c>
+      <c r="F25" s="1">
         <v>84.75</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
@@ -1898,11 +2007,15 @@
       <c r="D26" s="1">
         <v>51941.17</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="2">
+        <f t="shared" si="0"/>
+        <v>10.857867010954562</v>
+      </c>
+      <c r="F26" s="1">
         <v>85.23</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -1915,11 +2028,15 @@
       <c r="D27" s="1">
         <v>55727.72</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="2">
+        <f t="shared" si="0"/>
+        <v>10.928232968188912</v>
+      </c>
+      <c r="F27" s="1">
         <v>84.52</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
@@ -1932,11 +2049,15 @@
       <c r="D28" s="1">
         <v>47025.43</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="2">
+        <f t="shared" si="0"/>
+        <v>10.758443798199727</v>
+      </c>
+      <c r="F28" s="1">
         <v>83.71</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>59</v>
       </c>
@@ -1949,11 +2070,15 @@
       <c r="D29" s="1">
         <v>50232.2</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="2">
+        <f t="shared" si="0"/>
+        <v>10.824411534311739</v>
+      </c>
+      <c r="F29" s="1">
         <v>83.18</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>61</v>
       </c>
@@ -1966,11 +2091,15 @@
       <c r="D30" s="1">
         <v>48318.89</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="2">
+        <f t="shared" si="0"/>
+        <v>10.785577860490536</v>
+      </c>
+      <c r="F30" s="1">
         <v>83.17</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>63</v>
       </c>
@@ -1983,11 +2112,15 @@
       <c r="D31" s="1">
         <v>71308.92</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="2">
+        <f t="shared" si="0"/>
+        <v>11.174776703766726</v>
+      </c>
+      <c r="F31" s="1">
         <v>84.65</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>65</v>
       </c>
@@ -2000,11 +2133,15 @@
       <c r="D32" s="1">
         <v>38116.36</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="2">
+        <f t="shared" si="0"/>
+        <v>10.548398865276033</v>
+      </c>
+      <c r="F32" s="1">
         <v>82.46</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>67</v>
       </c>
@@ -2017,11 +2154,15 @@
       <c r="D33" s="1">
         <v>43661.54</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="2">
+        <f t="shared" si="0"/>
+        <v>10.684222902042569</v>
+      </c>
+      <c r="F33" s="1">
         <v>80.17</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>69</v>
       </c>
@@ -2034,11 +2175,15 @@
       <c r="D34" s="1">
         <v>38566.29</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="2">
+        <f t="shared" si="0"/>
+        <v>10.560133857828108</v>
+      </c>
+      <c r="F34" s="1">
         <v>81.290000000000006</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>71</v>
       </c>
@@ -2051,11 +2196,15 @@
       <c r="D35" s="1">
         <v>35328.79</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="2">
+        <f t="shared" si="0"/>
+        <v>10.472453491252686</v>
+      </c>
+      <c r="F35" s="1">
         <v>82.44</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>73</v>
       </c>
@@ -2068,11 +2217,15 @@
       <c r="D36" s="1">
         <v>29691.19</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="2">
+        <f t="shared" si="0"/>
+        <v>10.298605647789888</v>
+      </c>
+      <c r="F36" s="1">
         <v>80.78</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>75</v>
       </c>
@@ -2085,11 +2238,15 @@
       <c r="D37" s="1">
         <v>39538.49</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="2">
+        <f t="shared" si="0"/>
+        <v>10.585029906819864</v>
+      </c>
+      <c r="F37" s="1">
         <v>82.32</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>77</v>
       </c>
@@ -2102,11 +2259,15 @@
       <c r="D38" s="1">
         <v>30983.69</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="2">
+        <f t="shared" si="0"/>
+        <v>10.34121621598058</v>
+      </c>
+      <c r="F38" s="1">
         <v>80.27</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>79</v>
       </c>
@@ -2119,11 +2280,15 @@
       <c r="D39" s="1">
         <v>24650.49</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="2">
+        <f t="shared" si="0"/>
+        <v>10.112552057569411</v>
+      </c>
+      <c r="F39" s="1">
         <v>80.650000000000006</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
@@ -2136,11 +2301,15 @@
       <c r="D40" s="1">
         <v>40683.879999999997</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="2">
+        <f t="shared" si="0"/>
+        <v>10.613587224178655</v>
+      </c>
+      <c r="F40" s="1">
         <v>78.209999999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>83</v>
       </c>
@@ -2153,11 +2322,15 @@
       <c r="D41" s="1">
         <v>27127.439999999999</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="2">
+        <f t="shared" si="0"/>
+        <v>10.208301040714201</v>
+      </c>
+      <c r="F41" s="1">
         <v>78.64</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>85</v>
       </c>
@@ -2170,11 +2343,15 @@
       <c r="D42" s="1">
         <v>16325.46</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="2">
+        <f t="shared" si="0"/>
+        <v>9.7004811313893029</v>
+      </c>
+      <c r="F42" s="1">
         <v>79.599999999999994</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>87</v>
       </c>
@@ -2187,11 +2364,15 @@
       <c r="D43" s="1">
         <v>32511.83</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="2">
+        <f t="shared" si="0"/>
+        <v>10.3893593020859</v>
+      </c>
+      <c r="F43" s="1">
         <v>76.81</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>89</v>
       </c>
@@ -2205,11 +2386,15 @@
         <f>29.95*1000</f>
         <v>29950</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="2">
+        <f t="shared" si="0"/>
+        <v>10.307284603543595</v>
+      </c>
+      <c r="F44" s="1">
         <v>74.06</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>91</v>
       </c>
@@ -2222,11 +2407,15 @@
       <c r="D45" s="1">
         <v>39872.449999999997</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="2">
+        <f t="shared" si="0"/>
+        <v>10.593440888199007</v>
+      </c>
+      <c r="F45" s="1">
         <v>76.89</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>93</v>
       </c>
@@ -2239,11 +2428,15 @@
       <c r="D46" s="1">
         <v>32735.4</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="2">
+        <f t="shared" si="0"/>
+        <v>10.396212340137637</v>
+      </c>
+      <c r="F46" s="1">
         <v>74.08</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>95</v>
       </c>
@@ -2256,11 +2449,15 @@
       <c r="D47" s="1">
         <v>26166.05</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="2">
+        <f t="shared" si="0"/>
+        <v>10.172218047945705</v>
+      </c>
+      <c r="F47" s="1">
         <v>74.64</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>97</v>
       </c>
@@ -2273,11 +2470,15 @@
       <c r="D48" s="1">
         <v>23741.21</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="2">
+        <f t="shared" si="0"/>
+        <v>10.074967635693772</v>
+      </c>
+      <c r="F48" s="1">
         <v>75.8</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
@@ -2290,11 +2491,15 @@
       <c r="D49" s="1">
         <v>73724.31</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="2">
+        <f t="shared" si="0"/>
+        <v>11.208087874534899</v>
+      </c>
+      <c r="F49" s="1">
         <v>70.7</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>101</v>
       </c>
@@ -2307,11 +2512,15 @@
       <c r="D50" s="1">
         <v>113157.23</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="2">
+        <f t="shared" si="0"/>
+        <v>11.636533546501546</v>
+      </c>
+      <c r="F50" s="1">
         <v>66.47</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>103</v>
       </c>
@@ -2324,11 +2533,15 @@
       <c r="D51" s="1">
         <v>20612.189999999999</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="2">
+        <f t="shared" si="0"/>
+        <v>9.9336379273369317</v>
+      </c>
+      <c r="F51" s="1">
         <v>74.430000000000007</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>105</v>
       </c>
@@ -2341,11 +2554,15 @@
       <c r="D52" s="1">
         <v>19100.25</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52" s="2">
+        <f t="shared" si="0"/>
+        <v>9.8574567029542965</v>
+      </c>
+      <c r="F52" s="1">
         <v>74.78</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>107</v>
       </c>
@@ -2358,11 +2575,15 @@
       <c r="D53" s="1">
         <v>24831.53</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="2">
+        <f t="shared" si="0"/>
+        <v>10.119869495613102</v>
+      </c>
+      <c r="F53" s="1">
         <v>75.44</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>109</v>
       </c>
@@ -2375,11 +2596,15 @@
       <c r="D54" s="1">
         <v>33790.400000000001</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54" s="2">
+        <f t="shared" si="0"/>
+        <v>10.42793201746011</v>
+      </c>
+      <c r="F54" s="1">
         <v>74.02</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>111</v>
       </c>
@@ -2392,11 +2617,15 @@
       <c r="D55" s="1">
         <v>17847.330000000002</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E55" s="2">
+        <f t="shared" si="0"/>
+        <v>9.7896091961876746</v>
+      </c>
+      <c r="F55" s="1">
         <v>71.260000000000005</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>113</v>
       </c>
@@ -2409,11 +2638,15 @@
       <c r="D56" s="1">
         <v>15229.46</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E56" s="2">
+        <f t="shared" si="0"/>
+        <v>9.6309869889244375</v>
+      </c>
+      <c r="F56" s="1">
         <v>74.19</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>115</v>
       </c>
@@ -2426,11 +2659,15 @@
       <c r="D57" s="1">
         <v>10113.969999999999</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57" s="2">
+        <f t="shared" si="0"/>
+        <v>9.2216729154500445</v>
+      </c>
+      <c r="F57" s="1">
         <v>73.48</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>117</v>
       </c>
@@ -2443,11 +2680,15 @@
       <c r="D58" s="1">
         <v>34210.879999999997</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58" s="2">
+        <f t="shared" si="0"/>
+        <v>10.440299001113477</v>
+      </c>
+      <c r="F58" s="1">
         <v>71.209999999999994</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>119</v>
       </c>
@@ -2460,11 +2701,15 @@
       <c r="D59" s="1">
         <v>40114.01</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E59" s="2">
+        <f t="shared" si="0"/>
+        <v>10.599480928835487</v>
+      </c>
+      <c r="F59" s="1">
         <v>67.7</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>121</v>
       </c>
@@ -2477,11 +2722,15 @@
       <c r="D60" s="1">
         <v>17261.03</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60" s="2">
+        <f t="shared" si="0"/>
+        <v>9.7562066384073098</v>
+      </c>
+      <c r="F60" s="1">
         <v>74.12</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>123</v>
       </c>
@@ -2494,11 +2743,15 @@
       <c r="D61" s="1">
         <v>13102.32</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E61" s="2">
+        <f t="shared" si="0"/>
+        <v>9.480544592745666</v>
+      </c>
+      <c r="F61" s="1">
         <v>68.180000000000007</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>125</v>
       </c>
@@ -2511,11 +2764,15 @@
       <c r="D62" s="1">
         <v>20751.66</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62" s="2">
+        <f t="shared" si="0"/>
+        <v>9.9403815224590151</v>
+      </c>
+      <c r="F62" s="1">
         <v>69.8</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>127</v>
       </c>
@@ -2528,11 +2785,15 @@
       <c r="D63" s="1">
         <v>14950.5</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E63" s="2">
+        <f t="shared" si="0"/>
+        <v>9.6125000230756203</v>
+      </c>
+      <c r="F63" s="1">
         <v>74.17</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>129</v>
       </c>
@@ -2545,11 +2806,15 @@
       <c r="D64" s="1">
         <v>20403.310000000001</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E64" s="2">
+        <f t="shared" si="0"/>
+        <v>9.9234524215723656</v>
+      </c>
+      <c r="F64" s="1">
         <v>72.739999999999995</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>131</v>
       </c>
@@ -2562,11 +2827,15 @@
       <c r="D65" s="1">
         <v>27942.69</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65" s="2">
+        <f t="shared" si="0"/>
+        <v>10.237910905914559</v>
+      </c>
+      <c r="F65" s="1">
         <v>75.58</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>133</v>
       </c>
@@ -2579,11 +2848,15 @@
       <c r="D66" s="1">
         <v>26526.639999999999</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E66" s="2">
+        <f t="shared" si="0"/>
+        <v>10.185904790034597</v>
+      </c>
+      <c r="F66" s="1">
         <v>71.489999999999995</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>135</v>
       </c>
@@ -2596,11 +2869,15 @@
       <c r="D67" s="1">
         <v>21393.72</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E67" s="2">
+        <f t="shared" ref="E67:E130" si="1">LN(D67)</f>
+        <v>9.9708526999988099</v>
+      </c>
+      <c r="F67" s="1">
         <v>68.02</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>137</v>
       </c>
@@ -2613,11 +2890,15 @@
       <c r="D68" s="1">
         <v>18732.72</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68" s="2">
+        <f t="shared" si="1"/>
+        <v>9.838027006464177</v>
+      </c>
+      <c r="F68" s="1">
         <v>69.83</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>139</v>
       </c>
@@ -2630,11 +2911,15 @@
       <c r="D69" s="1">
         <v>19355.669999999998</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69" s="2">
+        <f t="shared" si="1"/>
+        <v>9.8707406787908116</v>
+      </c>
+      <c r="F69" s="1">
         <v>71.23</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>141</v>
       </c>
@@ -2647,11 +2932,15 @@
       <c r="D70" s="1">
         <v>21809.59</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70" s="2">
+        <f t="shared" si="1"/>
+        <v>9.9901050603027919</v>
+      </c>
+      <c r="F70" s="1">
         <v>70.84</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>143</v>
       </c>
@@ -2664,11 +2953,15 @@
       <c r="D71" s="1">
         <v>56646.43</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71" s="2">
+        <f t="shared" si="1"/>
+        <v>10.944584245935538</v>
+      </c>
+      <c r="F71" s="1">
         <v>66.09</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>145</v>
       </c>
@@ -2681,11 +2974,15 @@
       <c r="D72" s="1">
         <v>21019.46</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="2">
+        <f t="shared" si="1"/>
+        <v>9.953203954281733</v>
+      </c>
+      <c r="F72" s="1">
         <v>65.739999999999995</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>147</v>
       </c>
@@ -2698,11 +2995,15 @@
       <c r="D73" s="1">
         <v>15198.23</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73" s="2">
+        <f t="shared" si="1"/>
+        <v>9.6289342526854256</v>
+      </c>
+      <c r="F73" s="1">
         <v>68.959999999999994</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>149</v>
       </c>
@@ -2713,9 +3014,9 @@
         <v>68.67</v>
       </c>
       <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>151</v>
       </c>
@@ -2728,11 +3029,15 @@
       <c r="D75" s="1">
         <v>13530.4</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75" s="2">
+        <f t="shared" si="1"/>
+        <v>9.5126942846598315</v>
+      </c>
+      <c r="F75" s="1">
         <v>71.75</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>153</v>
       </c>
@@ -2745,11 +3050,15 @@
       <c r="D76" s="1">
         <v>8447.5499999999993</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E76" s="2">
+        <f t="shared" si="1"/>
+        <v>9.0416317374818487</v>
+      </c>
+      <c r="F76" s="1">
         <v>66.12</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>155</v>
       </c>
@@ -2762,11 +3071,15 @@
       <c r="D77" s="1">
         <v>38128.69</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E77" s="2">
+        <f t="shared" si="1"/>
+        <v>10.548722296111411</v>
+      </c>
+      <c r="F77" s="1">
         <v>71.989999999999995</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>157</v>
       </c>
@@ -2779,11 +3092,15 @@
       <c r="D78" s="1">
         <v>22761.27</v>
       </c>
-      <c r="E78" s="1">
+      <c r="E78" s="2">
+        <f t="shared" si="1"/>
+        <v>10.032815686332031</v>
+      </c>
+      <c r="F78" s="1">
         <v>69.760000000000005</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>159</v>
       </c>
@@ -2796,11 +3113,15 @@
       <c r="D79" s="1">
         <v>51246.400000000001</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E79" s="2">
+        <f t="shared" si="1"/>
+        <v>10.844400650630996</v>
+      </c>
+      <c r="F79" s="1">
         <v>63.89</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>161</v>
       </c>
@@ -2813,11 +3134,15 @@
       <c r="D80" s="1">
         <v>9222.52</v>
       </c>
-      <c r="E80" s="1">
+      <c r="E80" s="2">
+        <f t="shared" si="1"/>
+        <v>9.1294035980778592</v>
+      </c>
+      <c r="F80" s="1">
         <v>67.319999999999993</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>163</v>
       </c>
@@ -2830,11 +3155,15 @@
       <c r="D81" s="1">
         <v>5991.54</v>
       </c>
-      <c r="E81" s="1">
+      <c r="E81" s="2">
+        <f t="shared" si="1"/>
+        <v>8.698103753224796</v>
+      </c>
+      <c r="F81" s="1">
         <v>67.23</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>165</v>
       </c>
@@ -2847,11 +3176,15 @@
       <c r="D82" s="1">
         <v>13495.53</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E82" s="2">
+        <f t="shared" si="1"/>
+        <v>9.5101137984860227</v>
+      </c>
+      <c r="F82" s="1">
         <v>66.67</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>167</v>
       </c>
@@ -2864,11 +3197,15 @@
       <c r="D83" s="1">
         <v>33061.06</v>
       </c>
-      <c r="E83" s="1">
+      <c r="E83" s="2">
+        <f t="shared" si="1"/>
+        <v>10.406111433776921</v>
+      </c>
+      <c r="F83" s="1">
         <v>66.59</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>169</v>
       </c>
@@ -2881,11 +3218,15 @@
       <c r="D84" s="1">
         <v>15102.57</v>
       </c>
-      <c r="E84" s="1">
+      <c r="E84" s="2">
+        <f t="shared" si="1"/>
+        <v>9.6226202069963609</v>
+      </c>
+      <c r="F84" s="1">
         <v>70.7</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>171</v>
       </c>
@@ -2898,11 +3239,15 @@
       <c r="D85" s="1">
         <v>7633.8</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E85" s="2">
+        <f t="shared" si="1"/>
+        <v>8.9403410343767096</v>
+      </c>
+      <c r="F85" s="1">
         <v>69.010000000000005</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>173</v>
       </c>
@@ -2915,11 +3260,15 @@
       <c r="D86" s="1">
         <v>9325.68</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E86" s="2">
+        <f t="shared" si="1"/>
+        <v>9.1405271641053289</v>
+      </c>
+      <c r="F86" s="1">
         <v>67.459999999999994</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>175</v>
       </c>
@@ -2932,11 +3281,15 @@
       <c r="D87" s="1">
         <v>13423.43</v>
       </c>
-      <c r="E87" s="1">
+      <c r="E87" s="2">
+        <f t="shared" si="1"/>
+        <v>9.5047569665420735</v>
+      </c>
+      <c r="F87" s="1">
         <v>68.05</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>177</v>
       </c>
@@ -2949,11 +3302,15 @@
       <c r="D88" s="1">
         <v>14322.33</v>
       </c>
-      <c r="E88" s="1">
+      <c r="E88" s="2">
+        <f t="shared" si="1"/>
+        <v>9.5695751367760895</v>
+      </c>
+      <c r="F88" s="1">
         <v>69.95</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>179</v>
       </c>
@@ -2966,11 +3323,15 @@
       <c r="D89" s="1">
         <v>15469.84</v>
       </c>
-      <c r="E89" s="1">
+      <c r="E89" s="2">
+        <f t="shared" si="1"/>
+        <v>9.646647600915049</v>
+      </c>
+      <c r="F89" s="1">
         <v>67.209999999999994</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>181</v>
       </c>
@@ -2983,11 +3344,15 @@
       <c r="D90" s="1">
         <v>13172.06</v>
       </c>
-      <c r="E90" s="1">
+      <c r="E90" s="2">
+        <f t="shared" si="1"/>
+        <v>9.4858531986027952</v>
+      </c>
+      <c r="F90" s="1">
         <v>69.22</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>183</v>
       </c>
@@ -3000,11 +3365,15 @@
       <c r="D91" s="1">
         <v>18741.740000000002</v>
       </c>
-      <c r="E91" s="1">
+      <c r="E91" s="2">
+        <f t="shared" si="1"/>
+        <v>9.8385084010019082</v>
+      </c>
+      <c r="F91" s="1">
         <v>71.22</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>185</v>
       </c>
@@ -3017,11 +3386,15 @@
       <c r="D92" s="1">
         <v>12328.55</v>
       </c>
-      <c r="E92" s="1">
+      <c r="E92" s="2">
+        <f t="shared" si="1"/>
+        <v>9.4196729898918683</v>
+      </c>
+      <c r="F92" s="1">
         <v>69.77</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>187</v>
       </c>
@@ -3034,11 +3407,15 @@
       <c r="D93" s="1">
         <v>12643.93</v>
       </c>
-      <c r="E93" s="1">
+      <c r="E93" s="2">
+        <f t="shared" si="1"/>
+        <v>9.4449325370974684</v>
+      </c>
+      <c r="F93" s="1">
         <v>67.02</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>189</v>
       </c>
@@ -3051,11 +3428,15 @@
       <c r="D94" s="1">
         <v>11860.06</v>
       </c>
-      <c r="E94" s="1">
+      <c r="E94" s="2">
+        <f t="shared" si="1"/>
+        <v>9.3809317315608425</v>
+      </c>
+      <c r="F94" s="1">
         <v>66.48</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>191</v>
       </c>
@@ -3068,11 +3449,15 @@
       <c r="D95" s="1">
         <v>63379</v>
       </c>
-      <c r="E95" s="1">
+      <c r="E95" s="2">
+        <f t="shared" si="1"/>
+        <v>11.056887855272539</v>
+      </c>
+      <c r="F95" s="1">
         <v>65.59</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>193</v>
       </c>
@@ -3085,11 +3470,15 @@
       <c r="D96" s="1">
         <v>9565.32</v>
       </c>
-      <c r="E96" s="1">
+      <c r="E96" s="2">
+        <f t="shared" si="1"/>
+        <v>9.165899336620539</v>
+      </c>
+      <c r="F96" s="1">
         <v>67.150000000000006</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>195</v>
       </c>
@@ -3102,11 +3491,15 @@
       <c r="D97" s="1">
         <v>21031.5</v>
       </c>
-      <c r="E97" s="1">
+      <c r="E97" s="2">
+        <f t="shared" si="1"/>
+        <v>9.9537765928292963</v>
+      </c>
+      <c r="F97" s="1">
         <v>63.26</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>197</v>
       </c>
@@ -3119,11 +3512,15 @@
       <c r="D98" s="1">
         <v>37667.769999999997</v>
       </c>
-      <c r="E98" s="1">
+      <c r="E98" s="2">
+        <f t="shared" si="1"/>
+        <v>10.536560100632762</v>
+      </c>
+      <c r="F98" s="1">
         <v>65.540000000000006</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>199</v>
       </c>
@@ -3136,11 +3533,15 @@
       <c r="D99" s="1">
         <v>17334.88</v>
       </c>
-      <c r="E99" s="1">
+      <c r="E99" s="2">
+        <f t="shared" si="1"/>
+        <v>9.7604759356838571</v>
+      </c>
+      <c r="F99" s="1">
         <v>65.89</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>201</v>
       </c>
@@ -3153,11 +3554,15 @@
       <c r="D100" s="1">
         <v>11103.49</v>
       </c>
-      <c r="E100" s="1">
+      <c r="E100" s="2">
+        <f t="shared" si="1"/>
+        <v>9.3150147522969853</v>
+      </c>
+      <c r="F100" s="1">
         <v>64.42</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>203</v>
       </c>
@@ -3170,11 +3575,15 @@
       <c r="D101" s="1">
         <v>8599.82</v>
       </c>
-      <c r="E101" s="1">
+      <c r="E101" s="2">
+        <f t="shared" si="1"/>
+        <v>9.0594965517899997</v>
+      </c>
+      <c r="F101" s="1">
         <v>64.040000000000006</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>205</v>
       </c>
@@ -3187,11 +3596,15 @@
       <c r="D102" s="1">
         <v>15499.91</v>
       </c>
-      <c r="E102" s="1">
+      <c r="E102" s="2">
+        <f t="shared" si="1"/>
+        <v>9.6485894964388681</v>
+      </c>
+      <c r="F102" s="1">
         <v>63.72</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>207</v>
       </c>
@@ -3202,11 +3615,11 @@
         <v>60.63</v>
       </c>
       <c r="D103" s="1"/>
-      <c r="E103" s="1">
+      <c r="F103" s="1">
         <v>56.75</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>209</v>
       </c>
@@ -3219,11 +3632,15 @@
       <c r="D104" s="1">
         <v>6616.12</v>
       </c>
-      <c r="E104" s="1">
+      <c r="E104" s="2">
+        <f t="shared" si="1"/>
+        <v>8.7972643743866801</v>
+      </c>
+      <c r="F104" s="1">
         <v>64.8</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>211</v>
       </c>
@@ -3236,11 +3653,15 @@
       <c r="D105" s="1">
         <v>6440.42</v>
       </c>
-      <c r="E105" s="1">
+      <c r="E105" s="2">
+        <f t="shared" si="1"/>
+        <v>8.7703490343631412</v>
+      </c>
+      <c r="F105" s="1">
         <v>61.17</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>213</v>
       </c>
@@ -3253,11 +3674,15 @@
       <c r="D106" s="1">
         <v>14777.56</v>
       </c>
-      <c r="E106" s="1">
+      <c r="E106" s="2">
+        <f t="shared" si="1"/>
+        <v>9.6008650929169779</v>
+      </c>
+      <c r="F106" s="1">
         <v>54.28</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>215</v>
       </c>
@@ -3270,11 +3695,15 @@
       <c r="D107" s="1">
         <v>12427.77</v>
       </c>
-      <c r="E107" s="1">
+      <c r="E107" s="2">
+        <f t="shared" si="1"/>
+        <v>9.427688763743685</v>
+      </c>
+      <c r="F107" s="1">
         <v>60.21</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>217</v>
       </c>
@@ -3287,11 +3716,15 @@
       <c r="D108" s="1">
         <v>11474.54</v>
       </c>
-      <c r="E108" s="1">
+      <c r="E108" s="2">
+        <f t="shared" si="1"/>
+        <v>9.3478859469792646</v>
+      </c>
+      <c r="F108" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>219</v>
       </c>
@@ -3302,11 +3735,11 @@
         <v>58.33</v>
       </c>
       <c r="D109" s="1"/>
-      <c r="E109" s="1">
+      <c r="F109" s="1">
         <v>58.62</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>221</v>
       </c>
@@ -3319,11 +3752,15 @@
       <c r="D110" s="1">
         <v>8568.59</v>
       </c>
-      <c r="E110" s="1">
+      <c r="E110" s="2">
+        <f t="shared" si="1"/>
+        <v>9.0558584706344671</v>
+      </c>
+      <c r="F110" s="1">
         <v>60.19</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>223</v>
       </c>
@@ -3336,11 +3773,15 @@
       <c r="D111" s="1">
         <v>5599.72</v>
       </c>
-      <c r="E111" s="1">
+      <c r="E111" s="2">
+        <f t="shared" si="1"/>
+        <v>8.6304718754731997</v>
+      </c>
+      <c r="F111" s="1">
         <v>62.49</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>225</v>
       </c>
@@ -3353,11 +3794,15 @@
       <c r="D112" s="1">
         <v>4310.8900000000003</v>
       </c>
-      <c r="E112" s="1">
+      <c r="E112" s="2">
+        <f t="shared" si="1"/>
+        <v>8.3688996583000428</v>
+      </c>
+      <c r="F112" s="1">
         <v>56.05</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>227</v>
       </c>
@@ -3370,11 +3815,15 @@
       <c r="D113" s="1">
         <v>7032.01</v>
       </c>
-      <c r="E113" s="1">
+      <c r="E113" s="2">
+        <f t="shared" si="1"/>
+        <v>8.8582278614345373</v>
+      </c>
+      <c r="F113" s="1">
         <v>60.23</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>229</v>
       </c>
@@ -3387,11 +3836,15 @@
       <c r="D114" s="1">
         <v>4632.83</v>
       </c>
-      <c r="E114" s="1">
+      <c r="E114" s="2">
+        <f t="shared" si="1"/>
+        <v>8.4409231914561467</v>
+      </c>
+      <c r="F114" s="1">
         <v>59.39</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>231</v>
       </c>
@@ -3404,11 +3857,15 @@
       <c r="D115" s="1">
         <v>16600.39</v>
       </c>
-      <c r="E115" s="1">
+      <c r="E115" s="2">
+        <f t="shared" si="1"/>
+        <v>9.7171814680445596</v>
+      </c>
+      <c r="F115" s="1">
         <v>58.73</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>233</v>
       </c>
@@ -3421,11 +3878,15 @@
       <c r="D116" s="1">
         <v>5454.21</v>
       </c>
-      <c r="E116" s="1">
+      <c r="E116" s="2">
+        <f t="shared" si="1"/>
+        <v>8.6041430665146645</v>
+      </c>
+      <c r="F116" s="1">
         <v>58.92</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>235</v>
       </c>
@@ -3438,11 +3899,15 @@
       <c r="D117" s="1">
         <v>13062</v>
       </c>
-      <c r="E117" s="1">
+      <c r="E117" s="2">
+        <f t="shared" si="1"/>
+        <v>9.4774625304626028</v>
+      </c>
+      <c r="F117" s="1">
         <v>56.82</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>237</v>
       </c>
@@ -3455,11 +3920,15 @@
       <c r="D118" s="1">
         <v>5513.86</v>
       </c>
-      <c r="E118" s="1">
+      <c r="E118" s="2">
+        <f t="shared" si="1"/>
+        <v>8.6150202013448371</v>
+      </c>
+      <c r="F118" s="1">
         <v>57.96</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>239</v>
       </c>
@@ -3472,11 +3941,15 @@
       <c r="D119" s="1">
         <v>19718.259999999998</v>
       </c>
-      <c r="E119" s="1">
+      <c r="E119" s="2">
+        <f t="shared" si="1"/>
+        <v>9.8893003889695468</v>
+      </c>
+      <c r="F119" s="1">
         <v>62.18</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>241</v>
       </c>
@@ -3489,11 +3962,15 @@
       <c r="D120" s="1">
         <v>4860.45</v>
       </c>
-      <c r="E120" s="1">
+      <c r="E120" s="2">
+        <f t="shared" si="1"/>
+        <v>8.4888863052007029</v>
+      </c>
+      <c r="F120" s="1">
         <v>55.71</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>243</v>
       </c>
@@ -3506,11 +3983,15 @@
       <c r="D121" s="1">
         <v>7805.15</v>
       </c>
-      <c r="E121" s="1">
+      <c r="E121" s="2">
+        <f t="shared" si="1"/>
+        <v>8.9625390512145717</v>
+      </c>
+      <c r="F121" s="1">
         <v>56.06</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>245</v>
       </c>
@@ -3523,11 +4004,15 @@
       <c r="D122" s="1">
         <v>4330.6499999999996</v>
       </c>
-      <c r="E122" s="1">
+      <c r="E122" s="2">
+        <f t="shared" si="1"/>
+        <v>8.3734729252037763</v>
+      </c>
+      <c r="F122" s="1">
         <v>57.7</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>247</v>
       </c>
@@ -3540,11 +4025,15 @@
       <c r="D123" s="1">
         <v>8215.1299999999992</v>
       </c>
-      <c r="E123" s="1">
+      <c r="E123" s="2">
+        <f t="shared" si="1"/>
+        <v>9.0137328550570537</v>
+      </c>
+      <c r="F123" s="1">
         <v>51.17</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>249</v>
       </c>
@@ -3557,11 +4046,15 @@
       <c r="D124" s="1">
         <v>2480.34</v>
       </c>
-      <c r="E124" s="1">
+      <c r="E124" s="2">
+        <f t="shared" si="1"/>
+        <v>7.8161509265363174</v>
+      </c>
+      <c r="F124" s="1">
         <v>52.4</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>251</v>
       </c>
@@ -3574,11 +4067,15 @@
       <c r="D125" s="1">
         <v>3504.15</v>
       </c>
-      <c r="E125" s="1">
+      <c r="E125" s="2">
+        <f t="shared" si="1"/>
+        <v>8.1617032593592143</v>
+      </c>
+      <c r="F125" s="1">
         <v>54.87</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>253</v>
       </c>
@@ -3591,11 +4088,15 @@
       <c r="D126" s="1">
         <v>5308.75</v>
       </c>
-      <c r="E126" s="1">
+      <c r="E126" s="2">
+        <f t="shared" si="1"/>
+        <v>8.5771116816274802</v>
+      </c>
+      <c r="F126" s="1">
         <v>51.46</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>255</v>
       </c>
@@ -3608,11 +4109,15 @@
       <c r="D127" s="1">
         <v>6699.91</v>
       </c>
-      <c r="E127" s="1">
+      <c r="E127" s="2">
+        <f t="shared" si="1"/>
+        <v>8.8098493724530158</v>
+      </c>
+      <c r="F127" s="1">
         <v>54.01</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>257</v>
       </c>
@@ -3625,11 +4130,15 @@
       <c r="D128" s="1">
         <v>3610.67</v>
       </c>
-      <c r="E128" s="1">
+      <c r="E128" s="2">
+        <f t="shared" si="1"/>
+        <v>8.1916486296740665</v>
+      </c>
+      <c r="F128" s="1">
         <v>52.07</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>259</v>
       </c>
@@ -3642,11 +4151,15 @@
       <c r="D129" s="1">
         <v>6135.85</v>
       </c>
-      <c r="E129" s="1">
+      <c r="E129" s="2">
+        <f t="shared" si="1"/>
+        <v>8.7219038968551956</v>
+      </c>
+      <c r="F129" s="1">
         <v>49.39</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>261</v>
       </c>
@@ -3659,11 +4172,15 @@
       <c r="D130" s="1">
         <v>3697.61</v>
       </c>
-      <c r="E130" s="1">
+      <c r="E130" s="2">
+        <f t="shared" si="1"/>
+        <v>8.2154419439734045</v>
+      </c>
+      <c r="F130" s="1">
         <v>55.59</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>263</v>
       </c>
@@ -3676,11 +4193,15 @@
       <c r="D131" s="1">
         <v>5669.96</v>
       </c>
-      <c r="E131" s="1">
+      <c r="E131" s="2">
+        <f t="shared" ref="E131:E171" si="2">LN(D131)</f>
+        <v>8.6429373420231919</v>
+      </c>
+      <c r="F131" s="1">
         <v>52.97</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>265</v>
       </c>
@@ -3693,11 +4214,15 @@
       <c r="D132" s="1">
         <v>2744.78</v>
       </c>
-      <c r="E132" s="1">
+      <c r="E132" s="2">
+        <f t="shared" si="2"/>
+        <v>7.917456205012301</v>
+      </c>
+      <c r="F132" s="1">
         <v>54.68</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>267</v>
       </c>
@@ -3710,11 +4235,15 @@
       <c r="D133" s="1">
         <v>2859.77</v>
       </c>
-      <c r="E133" s="1">
+      <c r="E133" s="2">
+        <f t="shared" si="2"/>
+        <v>7.958496480999651</v>
+      </c>
+      <c r="F133" s="1">
         <v>52.18</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>269</v>
       </c>
@@ -3727,11 +4256,15 @@
       <c r="D134" s="1">
         <v>5706.9</v>
       </c>
-      <c r="E134" s="1">
+      <c r="E134" s="2">
+        <f t="shared" si="2"/>
+        <v>8.6494312480422053</v>
+      </c>
+      <c r="F134" s="1">
         <v>51.32</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>271</v>
       </c>
@@ -3744,11 +4277,15 @@
       <c r="D135" s="1">
         <v>1703.6</v>
       </c>
-      <c r="E135" s="1">
+      <c r="E135" s="2">
+        <f t="shared" si="2"/>
+        <v>7.4404989380490587</v>
+      </c>
+      <c r="F135" s="1">
         <v>54.29</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>273</v>
       </c>
@@ -3761,11 +4298,15 @@
       <c r="D136" s="1">
         <v>10170.94</v>
       </c>
-      <c r="E136" s="1">
+      <c r="E136" s="2">
+        <f t="shared" si="2"/>
+        <v>9.2272899134832329</v>
+      </c>
+      <c r="F136" s="1">
         <v>49.19</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>275</v>
       </c>
@@ -3778,11 +4319,15 @@
       <c r="D137" s="1">
         <v>2769.18</v>
       </c>
-      <c r="E137" s="1">
+      <c r="E137" s="2">
+        <f t="shared" si="2"/>
+        <v>7.9263065264753196</v>
+      </c>
+      <c r="F137" s="1">
         <v>51.58</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>277</v>
       </c>
@@ -3795,11 +4340,15 @@
       <c r="D138" s="1">
         <v>3445.06</v>
       </c>
-      <c r="E138" s="1">
+      <c r="E138" s="2">
+        <f t="shared" si="2"/>
+        <v>8.1446965998418115</v>
+      </c>
+      <c r="F138" s="1">
         <v>52.11</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>279</v>
       </c>
@@ -3812,11 +4361,15 @@
       <c r="D139" s="1">
         <v>2457.4499999999998</v>
       </c>
-      <c r="E139" s="1">
+      <c r="E139" s="2">
+        <f t="shared" si="2"/>
+        <v>7.8068795059343818</v>
+      </c>
+      <c r="F139" s="1">
         <v>52.9</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>281</v>
       </c>
@@ -3829,11 +4382,15 @@
       <c r="D140" s="1">
         <v>2914.53</v>
       </c>
-      <c r="E140" s="1">
+      <c r="E140" s="2">
+        <f t="shared" si="2"/>
+        <v>7.9774638507934101</v>
+      </c>
+      <c r="F140" s="1">
         <v>51.98</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>283</v>
       </c>
@@ -3846,11 +4403,15 @@
       <c r="D141" s="1">
         <v>3420.03</v>
       </c>
-      <c r="E141" s="1">
+      <c r="E141" s="2">
+        <f t="shared" si="2"/>
+        <v>8.1374046019480026</v>
+      </c>
+      <c r="F141" s="1">
         <v>52.17</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>285</v>
       </c>
@@ -3863,11 +4424,15 @@
       <c r="D142" s="1">
         <v>4785.68</v>
       </c>
-      <c r="E142" s="1">
+      <c r="E142" s="2">
+        <f t="shared" si="2"/>
+        <v>8.4733834045530774</v>
+      </c>
+      <c r="F142" s="1">
         <v>51.4</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>287</v>
       </c>
@@ -3880,11 +4445,15 @@
       <c r="D143" s="1">
         <v>2728.55</v>
       </c>
-      <c r="E143" s="1">
+      <c r="E143" s="2">
+        <f t="shared" si="2"/>
+        <v>7.9115256115454287</v>
+      </c>
+      <c r="F143" s="1">
         <v>49.34</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>289</v>
       </c>
@@ -3897,11 +4466,15 @@
       <c r="D144" s="1">
         <v>7407.11</v>
       </c>
-      <c r="E144" s="1">
+      <c r="E144" s="2">
+        <f t="shared" si="2"/>
+        <v>8.9101956287198121</v>
+      </c>
+      <c r="F144" s="1">
         <v>46.87</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>291</v>
       </c>
@@ -3914,11 +4487,15 @@
       <c r="D145" s="1">
         <v>7462.57</v>
       </c>
-      <c r="E145" s="1">
+      <c r="E145" s="2">
+        <f t="shared" si="2"/>
+        <v>8.9176551378913693</v>
+      </c>
+      <c r="F145" s="1">
         <v>48.27</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>293</v>
       </c>
@@ -3931,11 +4508,15 @@
       <c r="D146" s="1">
         <v>4141.22</v>
       </c>
-      <c r="E146" s="1">
+      <c r="E146" s="2">
+        <f t="shared" si="2"/>
+        <v>8.3287457093983104</v>
+      </c>
+      <c r="F146" s="1">
         <v>48.12</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>295</v>
       </c>
@@ -3948,11 +4529,15 @@
       <c r="D147" s="1">
         <v>18165.16</v>
       </c>
-      <c r="E147" s="1">
+      <c r="E147" s="2">
+        <f t="shared" si="2"/>
+        <v>9.8072607527640479</v>
+      </c>
+      <c r="F147" s="1">
         <v>46.58</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>297</v>
       </c>
@@ -3965,11 +4550,15 @@
       <c r="D148" s="1">
         <v>2413.04</v>
       </c>
-      <c r="E148" s="1">
+      <c r="E148" s="2">
+        <f t="shared" si="2"/>
+        <v>7.7886426423628956</v>
+      </c>
+      <c r="F148" s="1">
         <v>46.93</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>299</v>
       </c>
@@ -3982,11 +4571,15 @@
       <c r="D149" s="1">
         <v>6207.05</v>
       </c>
-      <c r="E149" s="1">
+      <c r="E149" s="2">
+        <f t="shared" si="2"/>
+        <v>8.7334410218025074</v>
+      </c>
+      <c r="F149" s="1">
         <v>46.6</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>301</v>
       </c>
@@ -3999,11 +4592,15 @@
       <c r="D150" s="1">
         <v>2698.61</v>
       </c>
-      <c r="E150" s="1">
+      <c r="E150" s="2">
+        <f t="shared" si="2"/>
+        <v>7.9004921046149601</v>
+      </c>
+      <c r="F150" s="1">
         <v>47.43</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>303</v>
       </c>
@@ -4016,11 +4613,15 @@
       <c r="D151" s="1">
         <v>2192.42</v>
       </c>
-      <c r="E151" s="1">
+      <c r="E151" s="2">
+        <f t="shared" si="2"/>
+        <v>7.6927612355532675</v>
+      </c>
+      <c r="F151" s="1">
         <v>46.65</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>305</v>
       </c>
@@ -4033,11 +4634,15 @@
       <c r="D152" s="1">
         <v>1598.18</v>
       </c>
-      <c r="E152" s="1">
+      <c r="E152" s="2">
+        <f t="shared" si="2"/>
+        <v>7.3766207607837222</v>
+      </c>
+      <c r="F152" s="1">
         <v>49.03</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>307</v>
       </c>
@@ -4050,11 +4655,15 @@
       <c r="D153" s="1">
         <v>2448.13</v>
       </c>
-      <c r="E153" s="1">
+      <c r="E153" s="2">
+        <f t="shared" si="2"/>
+        <v>7.8030797467973825</v>
+      </c>
+      <c r="F153" s="1">
         <v>49.83</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>309</v>
       </c>
@@ -4067,11 +4676,15 @@
       <c r="D154" s="1">
         <v>3299.88</v>
       </c>
-      <c r="E154" s="1">
+      <c r="E154" s="2">
+        <f t="shared" si="2"/>
+        <v>8.1016413831570357</v>
+      </c>
+      <c r="F154" s="1">
         <v>45.41</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>311</v>
       </c>
@@ -4084,11 +4697,15 @@
       <c r="D155" s="1">
         <v>1643.99</v>
       </c>
-      <c r="E155" s="1">
+      <c r="E155" s="2">
+        <f t="shared" si="2"/>
+        <v>7.4048814928725646</v>
+      </c>
+      <c r="F155" s="1">
         <v>50.48</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>313</v>
       </c>
@@ -4101,11 +4718,15 @@
       <c r="D156" s="1">
         <v>6272.33</v>
       </c>
-      <c r="E156" s="1">
+      <c r="E156" s="2">
+        <f t="shared" si="2"/>
+        <v>8.7439031754420515</v>
+      </c>
+      <c r="F156" s="1">
         <v>47.54</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>315</v>
       </c>
@@ -4118,11 +4739,15 @@
       <c r="D157" s="1">
         <v>1664.58</v>
       </c>
-      <c r="E157" s="1">
+      <c r="E157" s="2">
+        <f t="shared" si="2"/>
+        <v>7.4173281183413415</v>
+      </c>
+      <c r="F157" s="1">
         <v>47.07</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>317</v>
       </c>
@@ -4133,11 +4758,11 @@
         <v>41.2</v>
       </c>
       <c r="D158" s="1"/>
-      <c r="E158" s="1">
+      <c r="F158" s="1">
         <v>39.08</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>319</v>
       </c>
@@ -4150,11 +4775,15 @@
       <c r="D159" s="1">
         <v>3818.25</v>
       </c>
-      <c r="E159" s="1">
+      <c r="E159" s="2">
+        <f t="shared" si="2"/>
+        <v>8.2475474814505549</v>
+      </c>
+      <c r="F159" s="1">
         <v>42.41</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>321</v>
       </c>
@@ -4167,11 +4796,15 @@
       <c r="D160" s="1">
         <v>857.17</v>
       </c>
-      <c r="E160" s="1">
+      <c r="E160" s="2">
+        <f t="shared" si="2"/>
+        <v>6.7536362653201669</v>
+      </c>
+      <c r="F160" s="1">
         <v>42.91</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>323</v>
       </c>
@@ -4184,11 +4817,15 @@
       <c r="D161" s="1">
         <v>1652.72</v>
       </c>
-      <c r="E161" s="1">
+      <c r="E161" s="2">
+        <f t="shared" si="2"/>
+        <v>7.410177694483373</v>
+      </c>
+      <c r="F161" s="1">
         <v>43.14</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>325</v>
       </c>
@@ -4201,11 +4838,15 @@
       <c r="D162" s="1">
         <v>3026.24</v>
       </c>
-      <c r="E162" s="1">
+      <c r="E162" s="2">
+        <f t="shared" si="2"/>
+        <v>8.0150762038271477</v>
+      </c>
+      <c r="F162" s="1">
         <v>45.42</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>327</v>
       </c>
@@ -4218,11 +4859,15 @@
       <c r="D163" s="1">
         <v>1452.27</v>
       </c>
-      <c r="E163" s="1">
+      <c r="E163" s="2">
+        <f t="shared" si="2"/>
+        <v>7.2808831285113298</v>
+      </c>
+      <c r="F163" s="1">
         <v>35.85</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>329</v>
       </c>
@@ -4233,11 +4878,11 @@
         <v>37.9</v>
       </c>
       <c r="D164" s="1"/>
-      <c r="E164" s="1">
+      <c r="F164" s="1">
         <v>34.85</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>331</v>
       </c>
@@ -4250,11 +4895,15 @@
       <c r="D165" s="1">
         <v>1432.86</v>
       </c>
-      <c r="E165" s="1">
+      <c r="E165" s="2">
+        <f t="shared" si="2"/>
+        <v>7.267427725916626</v>
+      </c>
+      <c r="F165" s="1">
         <v>42.7</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>333</v>
       </c>
@@ -4267,11 +4916,15 @@
       <c r="D166" s="1">
         <v>2138.87</v>
       </c>
-      <c r="E166" s="1">
+      <c r="E166" s="2">
+        <f t="shared" si="2"/>
+        <v>7.6680329311718847</v>
+      </c>
+      <c r="F166" s="1">
         <v>37.340000000000003</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>335</v>
       </c>
@@ -4284,11 +4937,15 @@
       <c r="D167" s="1">
         <v>1748.48</v>
       </c>
-      <c r="E167" s="1">
+      <c r="E167" s="2">
+        <f t="shared" si="2"/>
+        <v>7.4665021180622615</v>
+      </c>
+      <c r="F167" s="1">
         <v>34.69</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>337</v>
       </c>
@@ -4301,11 +4958,15 @@
       <c r="D168" s="1">
         <v>1039.27</v>
       </c>
-      <c r="E168" s="1">
+      <c r="E168" s="2">
+        <f t="shared" si="2"/>
+        <v>6.9462738225951535</v>
+      </c>
+      <c r="F168" s="1">
         <v>32.39</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>339</v>
       </c>
@@ -4316,41 +4977,33 @@
         <v>26.5</v>
       </c>
       <c r="D169" s="1"/>
-      <c r="E169" s="1">
+      <c r="F169" s="1">
         <v>30.65</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>341</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+      <c r="F170" s="1">
+        <v>65.19</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D170" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="E170" s="1">
-        <v>65.19</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A171" s="1" t="s">
+      <c r="B171" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B171" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="E171" s="1">
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="F171" s="1">
         <v>86.47</v>
       </c>
     </row>

</xml_diff>